<commit_message>
added PHPSpreadsheet to read excel data and limited upload to max 2
</commit_message>
<xml_diff>
--- a/uploads/1.xlsx
+++ b/uploads/1.xlsx
@@ -1,15 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27230"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ankushgoel/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -340,9 +353,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -375,9 +388,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -581,22 +594,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="50.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="130.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="94.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="94.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="50.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>57</v>
       </c>
@@ -621,9 +632,8 @@
       <c r="H1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="I1" s="7"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -649,7 +659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -675,7 +685,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -701,7 +711,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -727,7 +737,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -753,7 +763,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -779,7 +789,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -805,7 +815,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -831,7 +841,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -857,7 +867,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -883,7 +893,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -909,7 +919,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -935,7 +945,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -961,7 +971,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -987,7 +997,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>